<commit_message>
# update cash_hist and some tools.
</commit_message>
<xml_diff>
--- a/history/schedule.xlsx
+++ b/history/schedule.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="15" windowWidth="11700" windowHeight="6525"/>
+    <workbookView xWindow="9150" yWindow="6090" windowWidth="11700" windowHeight="6525"/>
   </bookViews>
   <sheets>
     <sheet name="May" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="22">
   <si>
     <t>status</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -70,6 +70,30 @@
   </si>
   <si>
     <t>showa</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>showa</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>showa</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>showa</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Meal Card:</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Week</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Day</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -77,10 +101,11 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="7" formatCode="&quot;￥&quot;#,##0.00;&quot;￥&quot;\-#,##0.00"/>
+    <numFmt numFmtId="176" formatCode="[$-409]d/mmm;@"/>
   </numFmts>
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -96,8 +121,15 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="宋体"/>
+      <family val="2"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -107,6 +139,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -125,7 +163,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -135,11 +173,17 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="58" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="7" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="7" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+    <xf numFmtId="7" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -435,18 +479,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:P35"/>
+  <dimension ref="A1:P36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
-    <col min="1" max="1" width="10.25" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16">
+      <c r="A1" s="6" t="s">
+        <v>20</v>
+      </c>
       <c r="B1" s="1" t="s">
         <v>7</v>
       </c>
@@ -494,49 +541,52 @@
       </c>
     </row>
     <row r="2" spans="1:16">
-      <c r="B2" s="3">
+      <c r="A2" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B2" s="4">
         <v>40680</v>
       </c>
-      <c r="C2" s="3">
+      <c r="C2" s="4">
         <v>40681</v>
       </c>
-      <c r="D2" s="3">
+      <c r="D2" s="4">
         <v>40682</v>
       </c>
-      <c r="E2" s="3">
+      <c r="E2" s="4">
         <v>40683</v>
       </c>
-      <c r="F2" s="3">
+      <c r="F2" s="4">
         <v>40684</v>
       </c>
-      <c r="G2" s="3">
+      <c r="G2" s="4">
         <v>40685</v>
       </c>
-      <c r="H2" s="3">
+      <c r="H2" s="4">
         <v>40686</v>
       </c>
-      <c r="I2" s="3">
+      <c r="I2" s="4">
         <v>40687</v>
       </c>
-      <c r="J2" s="3">
+      <c r="J2" s="4">
         <v>40688</v>
       </c>
-      <c r="K2" s="3">
+      <c r="K2" s="4">
         <v>40689</v>
       </c>
-      <c r="L2" s="3">
+      <c r="L2" s="4">
         <v>40690</v>
       </c>
-      <c r="M2" s="3">
+      <c r="M2" s="4">
         <v>40691</v>
       </c>
-      <c r="N2" s="3">
+      <c r="N2" s="4">
         <v>40692</v>
       </c>
-      <c r="O2" s="3">
+      <c r="O2" s="4">
         <v>40693</v>
       </c>
-      <c r="P2" s="3">
+      <c r="P2" s="4">
         <v>40694</v>
       </c>
     </row>
@@ -544,35 +594,139 @@
       <c r="A3" t="s">
         <v>0</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="1" t="s">
         <v>15</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:16">
       <c r="A4" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="4">
+      <c r="B4" s="3">
         <v>66</v>
       </c>
+      <c r="C4" s="3">
+        <v>64</v>
+      </c>
+      <c r="D4" s="3">
+        <v>68</v>
+      </c>
+      <c r="E4" s="5">
+        <v>9</v>
+      </c>
+      <c r="F4" s="3"/>
+      <c r="G4" s="3"/>
+      <c r="H4" s="3"/>
+      <c r="I4" s="3"/>
+      <c r="J4" s="3"/>
+      <c r="K4" s="3"/>
+      <c r="L4" s="3"/>
+      <c r="M4" s="3"/>
+      <c r="N4" s="3"/>
+      <c r="O4" s="3"/>
+      <c r="P4" s="3"/>
     </row>
     <row r="5" spans="1:16">
       <c r="A5" t="s">
-        <v>2</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="B5" s="3"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3">
+        <v>73</v>
+      </c>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3"/>
+      <c r="H5" s="3"/>
+      <c r="I5" s="3"/>
+      <c r="J5" s="3"/>
+      <c r="K5" s="3"/>
+      <c r="L5" s="3"/>
+      <c r="M5" s="3"/>
+      <c r="N5" s="3"/>
+      <c r="O5" s="3"/>
+      <c r="P5" s="3"/>
     </row>
     <row r="6" spans="1:16">
       <c r="A6" t="s">
-        <v>3</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="B6" s="3"/>
+      <c r="C6" s="3">
+        <v>18</v>
+      </c>
+      <c r="D6" s="3">
+        <v>12</v>
+      </c>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="3"/>
+      <c r="I6" s="3"/>
+      <c r="J6" s="3"/>
+      <c r="K6" s="3"/>
+      <c r="L6" s="3"/>
+      <c r="M6" s="3"/>
+      <c r="N6" s="3"/>
+      <c r="O6" s="3"/>
+      <c r="P6" s="3"/>
     </row>
     <row r="7" spans="1:16">
       <c r="A7" t="s">
+        <v>3</v>
+      </c>
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="3"/>
+      <c r="H7" s="3"/>
+      <c r="I7" s="3"/>
+      <c r="J7" s="3"/>
+      <c r="K7" s="3"/>
+      <c r="L7" s="3"/>
+      <c r="M7" s="3"/>
+      <c r="N7" s="3"/>
+      <c r="O7" s="3"/>
+      <c r="P7" s="3"/>
+    </row>
+    <row r="8" spans="1:16">
+      <c r="A8" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="35" spans="1:1">
-      <c r="A35" t="s">
+      <c r="B8" s="3"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="3"/>
+      <c r="H8" s="3"/>
+      <c r="I8" s="3"/>
+      <c r="J8" s="3"/>
+      <c r="K8" s="3"/>
+      <c r="L8" s="3"/>
+      <c r="M8" s="3"/>
+      <c r="N8" s="3"/>
+      <c r="O8" s="3"/>
+      <c r="P8" s="3"/>
+    </row>
+    <row r="9" spans="1:16">
+      <c r="A9" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1">
+      <c r="A36" t="s">
         <v>14</v>
       </c>
     </row>

</xml_diff>

<commit_message>
# update my life log.
</commit_message>
<xml_diff>
--- a/history/schedule.xlsx
+++ b/history/schedule.xlsx
@@ -13,8 +13,90 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>zy</author>
+  </authors>
+  <commentList>
+    <comment ref="E4" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t>与</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Jack</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t>重复打车</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C6" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t>华景新城</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>-&gt;</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t>岑村</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="22">
   <si>
     <t>status</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -105,7 +187,7 @@
     <numFmt numFmtId="7" formatCode="&quot;￥&quot;#,##0.00;&quot;￥&quot;\-#,##0.00"/>
     <numFmt numFmtId="176" formatCode="[$-409]d/mmm;@"/>
   </numFmts>
-  <fonts count="3">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -128,8 +210,23 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -148,6 +245,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -163,7 +266,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -184,6 +287,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="7" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="7" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -479,15 +588,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:P36"/>
+  <dimension ref="A1:P37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
     <col min="1" max="1" width="11.625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16">
@@ -606,6 +716,25 @@
       <c r="E3" s="1" t="s">
         <v>18</v>
       </c>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="I3" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="J3" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="K3" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="L3" s="8"/>
+      <c r="M3" s="8"/>
+      <c r="N3" s="8"/>
+      <c r="O3" s="8"/>
+      <c r="P3" s="8"/>
     </row>
     <row r="4" spans="1:16">
       <c r="A4" t="s">
@@ -628,7 +757,9 @@
       <c r="H4" s="3"/>
       <c r="I4" s="3"/>
       <c r="J4" s="3"/>
-      <c r="K4" s="3"/>
+      <c r="K4" s="3">
+        <v>53</v>
+      </c>
       <c r="L4" s="3"/>
       <c r="M4" s="3"/>
       <c r="N4" s="3"/>
@@ -662,7 +793,7 @@
         <v>2</v>
       </c>
       <c r="B6" s="3"/>
-      <c r="C6" s="3">
+      <c r="C6" s="7">
         <v>18</v>
       </c>
       <c r="D6" s="3">
@@ -670,9 +801,15 @@
       </c>
       <c r="F6" s="3"/>
       <c r="G6" s="3"/>
-      <c r="H6" s="3"/>
-      <c r="I6" s="3"/>
-      <c r="J6" s="3"/>
+      <c r="H6" s="3">
+        <v>13</v>
+      </c>
+      <c r="I6" s="3">
+        <v>12</v>
+      </c>
+      <c r="J6" s="3">
+        <v>12</v>
+      </c>
       <c r="K6" s="3"/>
       <c r="L6" s="3"/>
       <c r="M6" s="3"/>
@@ -687,13 +824,20 @@
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
       <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
       <c r="F7" s="3"/>
       <c r="G7" s="3"/>
-      <c r="H7" s="3"/>
-      <c r="I7" s="3"/>
-      <c r="J7" s="3"/>
-      <c r="K7" s="3"/>
+      <c r="H7" s="3">
+        <v>3</v>
+      </c>
+      <c r="I7" s="3">
+        <v>2</v>
+      </c>
+      <c r="J7" s="3">
+        <v>2</v>
+      </c>
+      <c r="K7" s="3">
+        <v>2</v>
+      </c>
       <c r="L7" s="3"/>
       <c r="M7" s="3"/>
       <c r="N7" s="3"/>
@@ -702,15 +846,16 @@
     </row>
     <row r="8" spans="1:16">
       <c r="A8" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
       <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
       <c r="F8" s="3"/>
       <c r="G8" s="3"/>
-      <c r="H8" s="3"/>
+      <c r="H8" s="3">
+        <v>25</v>
+      </c>
       <c r="I8" s="3"/>
       <c r="J8" s="3"/>
       <c r="K8" s="3"/>
@@ -722,11 +867,66 @@
     </row>
     <row r="9" spans="1:16">
       <c r="A9" t="s">
+        <v>4</v>
+      </c>
+      <c r="E9" s="3">
+        <v>25</v>
+      </c>
+      <c r="H9" s="3"/>
+      <c r="I9" s="3"/>
+      <c r="J9" s="3"/>
+      <c r="K9" s="3"/>
+      <c r="L9" s="3"/>
+      <c r="M9" s="3"/>
+      <c r="N9" s="3"/>
+      <c r="O9" s="3"/>
+      <c r="P9" s="3"/>
+    </row>
+    <row r="10" spans="1:16">
+      <c r="A10" t="s">
+        <v>4</v>
+      </c>
+      <c r="E10" s="3">
+        <v>2</v>
+      </c>
+      <c r="H10" s="3"/>
+      <c r="I10" s="3"/>
+      <c r="J10" s="3"/>
+      <c r="K10" s="3"/>
+      <c r="L10" s="3"/>
+      <c r="M10" s="3"/>
+      <c r="N10" s="3"/>
+      <c r="O10" s="3"/>
+      <c r="P10" s="3"/>
+    </row>
+    <row r="11" spans="1:16">
+      <c r="A11" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="36" spans="1:1">
-      <c r="A36" t="s">
+      <c r="H11" s="3"/>
+      <c r="I11" s="3">
+        <v>100</v>
+      </c>
+      <c r="K11" s="3"/>
+      <c r="L11" s="3"/>
+      <c r="M11" s="3"/>
+      <c r="N11" s="3"/>
+      <c r="O11" s="3"/>
+      <c r="P11" s="3"/>
+    </row>
+    <row r="12" spans="1:16">
+      <c r="H12" s="3"/>
+      <c r="I12" s="3"/>
+      <c r="J12" s="3"/>
+      <c r="K12" s="3"/>
+      <c r="L12" s="3"/>
+      <c r="M12" s="3"/>
+      <c r="N12" s="3"/>
+      <c r="O12" s="3"/>
+      <c r="P12" s="3"/>
+    </row>
+    <row r="37" spans="1:1">
+      <c r="A37" t="s">
         <v>14</v>
       </c>
     </row>
@@ -734,5 +934,6 @@
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
# update my history.
</commit_message>
<xml_diff>
--- a/history/schedule.xlsx
+++ b/history/schedule.xlsx
@@ -100,7 +100,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="52">
   <si>
     <t>status</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1289,20 +1289,20 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H10"/>
+  <dimension ref="A1:H18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="7" ySplit="1" topLeftCell="H2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="H1" sqref="H1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C11" sqref="C11"/>
+      <selection pane="bottomRight" activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
     <col min="1" max="1" width="9.5" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="9.5" customWidth="1"/>
-    <col min="6" max="6" width="15.875" customWidth="1"/>
+    <col min="6" max="6" width="9.375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="34.375" style="10" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="40.875" bestFit="1" customWidth="1"/>
   </cols>
@@ -1534,6 +1534,166 @@
         <v>25</v>
       </c>
     </row>
+    <row r="11" spans="1:8">
+      <c r="A11" s="9">
+        <v>40701</v>
+      </c>
+      <c r="B11" t="s">
+        <v>15</v>
+      </c>
+      <c r="C11" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="D11" t="s">
+        <v>41</v>
+      </c>
+      <c r="E11" t="s">
+        <v>45</v>
+      </c>
+      <c r="F11">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8">
+      <c r="A12" s="9">
+        <v>40701</v>
+      </c>
+      <c r="B12" t="s">
+        <v>15</v>
+      </c>
+      <c r="C12" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="D12" t="s">
+        <v>42</v>
+      </c>
+      <c r="E12" t="s">
+        <v>45</v>
+      </c>
+      <c r="F12">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8">
+      <c r="A13" s="9">
+        <v>40702</v>
+      </c>
+      <c r="B13" t="s">
+        <v>15</v>
+      </c>
+      <c r="C13" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="D13" t="s">
+        <v>41</v>
+      </c>
+      <c r="E13" t="s">
+        <v>45</v>
+      </c>
+      <c r="F13">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8">
+      <c r="A14" s="9">
+        <v>40702</v>
+      </c>
+      <c r="B14" t="s">
+        <v>15</v>
+      </c>
+      <c r="C14" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="D14" t="s">
+        <v>42</v>
+      </c>
+      <c r="E14" t="s">
+        <v>45</v>
+      </c>
+      <c r="F14">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8">
+      <c r="A15" s="9">
+        <v>40702</v>
+      </c>
+      <c r="B15" t="s">
+        <v>15</v>
+      </c>
+      <c r="C15" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="D15" t="s">
+        <v>41</v>
+      </c>
+      <c r="E15" t="s">
+        <v>45</v>
+      </c>
+      <c r="F15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8">
+      <c r="A16" s="9">
+        <v>40702</v>
+      </c>
+      <c r="B16" t="s">
+        <v>15</v>
+      </c>
+      <c r="C16" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="D16" t="s">
+        <v>42</v>
+      </c>
+      <c r="E16" t="s">
+        <v>45</v>
+      </c>
+      <c r="F16">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
+      <c r="A17" s="9">
+        <v>40703</v>
+      </c>
+      <c r="B17" t="s">
+        <v>15</v>
+      </c>
+      <c r="C17" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="D17" t="s">
+        <v>41</v>
+      </c>
+      <c r="E17" t="s">
+        <v>45</v>
+      </c>
+      <c r="F17">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
+      <c r="A18" s="9">
+        <v>40703</v>
+      </c>
+      <c r="B18" t="s">
+        <v>15</v>
+      </c>
+      <c r="C18" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="D18" t="s">
+        <v>42</v>
+      </c>
+      <c r="E18" t="s">
+        <v>45</v>
+      </c>
+      <c r="F18">
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:G1"/>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>